<commit_message>
Minor fixes and database module completed
</commit_message>
<xml_diff>
--- a/src/assets/files/subject-period.xlsx
+++ b/src/assets/files/subject-period.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiwa\Documents\Angular Projects\students-projects\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiwa\Documents\Angular Projects\students-projects-app\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28BBAD1-A4E3-4A32-9BE0-76DE19C98D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65B384E-1ED1-4A1F-9344-87745135F8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAF8C8D3-6278-4836-A629-04B0279E0A1C}"/>
   </bookViews>
@@ -104,14 +104,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,204 +430,204 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="3" width="20.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>